<commit_message>
Fix date handling Add bool and date tests
</commit_message>
<xml_diff>
--- a/ExcelMapper.Tests/Products.xlsx
+++ b/ExcelMapper.Tests/Products.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,12 @@
   </si>
   <si>
     <t>Number</t>
+  </si>
+  <si>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>OfferEnd</t>
   </si>
 </sst>
 </file>
@@ -82,12 +88,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Gut" xfId="1" builtinId="26"/>
@@ -390,15 +398,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="11.42578125" style="6"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -409,8 +420,14 @@
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -420,8 +437,11 @@
       <c r="D2" s="3">
         <v>1.99</v>
       </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -431,13 +451,19 @@
       <c r="D3" s="3">
         <v>2.99</v>
       </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>42369</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="C4" s="4"/>
       <c r="D4" s="3"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -446,6 +472,9 @@
       </c>
       <c r="D5" s="3">
         <v>0.99</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix #4 Update NuGet packages Implement VS suggestions
</commit_message>
<xml_diff>
--- a/ExcelMapper.Tests/Products.xlsx
+++ b/ExcelMapper.Tests/Products.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>OfferEnd</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -398,18 +401,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="11.42578125" style="6"/>
+    <col min="9" max="9" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -426,8 +430,15 @@
       <c r="F1" s="5" t="s">
         <v>7</v>
       </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="1">
+        <f>1+2</f>
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -443,8 +454,12 @@
       <c r="F2" s="6">
         <v>25569</v>
       </c>
+      <c r="G2" s="3">
+        <f>C2*D2</f>
+        <v>119.4</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -460,13 +475,18 @@
       <c r="F3" s="6">
         <v>42369</v>
       </c>
+      <c r="G3" s="3">
+        <f t="shared" ref="G3:G5" si="0">C3*D3</f>
+        <v>98.67</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="C4" s="4"/>
       <c r="D4" s="3"/>
+      <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -481,6 +501,10 @@
       </c>
       <c r="F5" s="6">
         <v>25569</v>
+      </c>
+      <c r="G5" s="3">
+        <f t="shared" si="0"/>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>